<commit_message>
taakverdeling ingevuld betreffende testdag
</commit_message>
<xml_diff>
--- a/uitvoering/taakverdeling.xlsx
+++ b/uitvoering/taakverdeling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomd\HoGent\3de JAAR\EP3\SEP\sep2324-gent-ep3\uitvoering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelle\Documents\Education\23-24\SEM3\SEP\sep2324-gent-ep3\uitvoering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1CDB66-9581-4747-8708-16DD2A4DE7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6593ABEB-0458-4C2A-8401-2AC080959B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>TAAK</t>
   </si>
@@ -60,13 +60,19 @@
     <t>Inhoudstabel README file</t>
   </si>
   <si>
-    <t>NAT portforwording en kleine aanpassingen in netwerkscripts toegevoegd</t>
-  </si>
-  <si>
     <t>Webserver, Databaseserver en reverseproxy aanpassingen in provisioningscript</t>
   </si>
   <si>
     <t>GPO toegevoegd</t>
+  </si>
+  <si>
+    <t>NAT portforwarding en kleine aanpassingen in netwerkscripts toegevoegd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fysieke testdag op school, focus op de totale test voor demo morgen en testen van laatste aanpassingen + test met ACLs actief. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA uitbreiding poging </t>
   </si>
 </sst>
 </file>
@@ -157,8 +163,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kop 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,16 +445,16 @@
   <dimension ref="B2:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="130.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="130.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -464,7 +470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -472,7 +478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -480,7 +486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
@@ -488,7 +494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
@@ -496,7 +502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
@@ -504,106 +510,116 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
     </row>
   </sheetData>

</xml_diff>